<commit_message>
Tạo thêm thư mục Test Plan và Test Design
</commit_message>
<xml_diff>
--- a/TestCase/TestCase_Organisation.xlsx
+++ b/TestCase/TestCase_Organisation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Tester_2023\Tester_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Tester_2023\Tester_2023\TestCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF8ED0E-1B5E-41BB-A561-CDA89DF7491F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDC0E2-8D15-4B5F-B125-D717AE64AD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{19E819FF-D694-4E47-9DEE-70124B6713EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{19E819FF-D694-4E47-9DEE-70124B6713EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -772,14 +772,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,13 +794,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,11 +811,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615823E2-1FDE-440B-B403-0AC79CAE0A83}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1189,54 +1189,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1255,11 +1255,11 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1268,9 +1268,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C54FCBA-7393-4349-8B3F-F9EB78175D6E}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.77734375" style="4" customWidth="1"/>
@@ -1538,55 +1538,55 @@
     <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1605,33 +1605,33 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1641,25 +1641,25 @@
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="6"/>
@@ -1669,7 +1669,7 @@
         <f>IF(OR(B9&lt;&gt;"", D9&lt;&gt;""), "[" &amp; TEXT($B$2, "##") &amp; "-" &amp; TEXT(ROW()-8, "##") &amp; "]", "")</f>
         <v>[Add Organisation-1]</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1788,20 +1788,19 @@
       <c r="H14" s="14"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="17" spans="4:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="13.8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F6:H6"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1809,13 +1808,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E71B9F9-90B6-4E04-97F6-7C1A4A3A198E}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.77734375" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.77734375" style="4" customWidth="1"/>
@@ -1828,55 +1827,55 @@
     <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1895,33 +1894,33 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -1931,25 +1930,25 @@
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="6"/>
@@ -1959,7 +1958,7 @@
         <f>IF(OR(B9&lt;&gt;"", D9&lt;&gt;""), "[" &amp; TEXT($B$2, "##") &amp; "-" &amp; TEXT(ROW()-8, "##") &amp; "]", "")</f>
         <v>[Amend Organisation-1]</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -2078,20 +2077,19 @@
       <c r="H14" s="14"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="17" spans="4:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="13.8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F6:H6"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>